<commit_message>
Agregar Codificacion del tipo de cuenta
</commit_message>
<xml_diff>
--- a/referencia/Codificacion ECR.xlsx
+++ b/referencia/Codificacion ECR.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GDrive\CP\SQL\ECR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zona Trabajo\SQL\BACK\ECR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0C3C3D-357D-4D8B-A0C1-951AC2B36D6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{04888224-15D9-43B9-B031-B1BF1D0C8D03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="CrsMessageTypeIndic_EnumType" sheetId="1" r:id="rId1"/>
-    <sheet name="CountryCode_Type" sheetId="2" r:id="rId2"/>
-    <sheet name="OECDDocTypeIndic_EnumType" sheetId="9" r:id="rId3"/>
-    <sheet name="OECDNameType_EnumType" sheetId="3" r:id="rId4"/>
-    <sheet name="OECDLegalAddressType_EnumType" sheetId="4" r:id="rId5"/>
-    <sheet name="CrsPaymentType_EnumType" sheetId="5" r:id="rId6"/>
-    <sheet name="currCode_Type" sheetId="6" r:id="rId7"/>
-    <sheet name="CtrlgPersonType" sheetId="7" r:id="rId8"/>
-    <sheet name="AcctHolderTypeCRS" sheetId="8" r:id="rId9"/>
+    <sheet name="AcctNumberType_EnumType" sheetId="10" r:id="rId1"/>
+    <sheet name="CrsMessageTypeIndic_EnumType" sheetId="1" r:id="rId2"/>
+    <sheet name="CountryCode_Type" sheetId="2" r:id="rId3"/>
+    <sheet name="OECDDocTypeIndic_EnumType" sheetId="9" r:id="rId4"/>
+    <sheet name="OECDNameType_EnumType" sheetId="3" r:id="rId5"/>
+    <sheet name="OECDLegalAddressType_EnumType" sheetId="4" r:id="rId6"/>
+    <sheet name="CrsPaymentType_EnumType" sheetId="5" r:id="rId7"/>
+    <sheet name="currCode_Type" sheetId="6" r:id="rId8"/>
+    <sheet name="CtrlgPersonType" sheetId="7" r:id="rId9"/>
+    <sheet name="AcctHolderTypeCRS" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">CtrlgPersonType!$A$3:$A$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">currCode_Type!$A$1:$D$269</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">CtrlgPersonType!$A$3:$A$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">currCode_Type!$A$1:$D$269</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="1185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="1201">
   <si>
     <t>CRS701</t>
   </si>
@@ -3598,12 +3598,60 @@
   </si>
   <si>
     <t>Deletion of Test Data</t>
+  </si>
+  <si>
+    <t>OECD601</t>
+  </si>
+  <si>
+    <t>OECD602</t>
+  </si>
+  <si>
+    <t>OECD603</t>
+  </si>
+  <si>
+    <t>OECD604</t>
+  </si>
+  <si>
+    <t>OECD605</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>OBAN</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>OSIN</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>International Bank Account Number</t>
+  </si>
+  <si>
+    <t>Other Bank Account Number</t>
+  </si>
+  <si>
+    <t>International Securities Information Number</t>
+  </si>
+  <si>
+    <t>Other Securities Information Number</t>
+  </si>
+  <si>
+    <t>Any Other type of account number</t>
+  </si>
+  <si>
+    <t>OBSER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3962,7 +4010,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D305011-4B2B-4B2F-B29A-93D09E9D5BAD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3999,8 +4179,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABA360D-9D9E-4BF4-8B28-98DE14F583A4}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B250"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6015,8 +6195,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43FEA4C-9473-416C-8873-9F05B7486041}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6106,11 +6286,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A96EC4-A752-4B7D-8ADA-E2994D4273EB}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -6197,8 +6377,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D394E625-D691-496F-BEAF-E5FD767BB4E9}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6261,12 +6441,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1062626-FC37-4F89-9DE8-0CB3CD9C1C3E}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6317,8 +6497,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70864208-5F0E-49D0-80B0-0CD51785B8EC}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9282,13 +9462,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D269" xr:uid="{03887261-43C3-4F73-8033-554D048E1492}"/>
+  <autoFilter ref="A1:D269"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FBF2F1-7FB6-462E-86BA-2ECC114075D8}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9417,54 +9597,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17ACCD09-F89B-49CB-AB13-5AFB74496957}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1137</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1138</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1139</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1142</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>